<commit_message>
Baseline production must be 0, if the system comes in later
</commit_message>
<xml_diff>
--- a/database/Steel Data Mar 10.xlsx
+++ b/database/Steel Data Mar 10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanghyun/Github/systempathway/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9191A49C-15BD-D348-A979-0C2D5932D433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBE6D98-804F-6F43-82C1-F13C0579BE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12540" yWindow="4740" windowWidth="50180" windowHeight="21880" tabRatio="775" activeTab="11" xr2:uid="{C8B88EB0-6E83-4E76-A7A7-49164EF16775}"/>
+    <workbookView xWindow="12540" yWindow="4740" windowWidth="50180" windowHeight="21880" tabRatio="775" activeTab="4" xr2:uid="{C8B88EB0-6E83-4E76-A7A7-49164EF16775}"/>
   </bookViews>
   <sheets>
     <sheet name="notes" sheetId="18" r:id="rId1"/>
@@ -1049,7 +1049,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1109,7 +1109,7 @@
         <v>20</v>
       </c>
       <c r="C4">
-        <v>2030</v>
+        <v>2020</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -1123,7 +1123,7 @@
         <v>20</v>
       </c>
       <c r="C5">
-        <v>2051</v>
+        <v>2020</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
@@ -1323,8 +1323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E46CCB1-2754-42FA-B5C9-8DABA83A320C}">
   <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10032,8 +10032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B80F836-AAFA-4D20-813C-A31BE68F85E1}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10381,10 +10381,10 @@
         <v>1</v>
       </c>
       <c r="G13" s="10">
-        <v>1683000</v>
+        <v>0</v>
       </c>
       <c r="H13" s="5">
-        <v>2010</v>
+        <v>2030</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -10407,10 +10407,10 @@
         <v>1</v>
       </c>
       <c r="G14" s="25">
-        <v>1280000</v>
+        <v>0</v>
       </c>
       <c r="H14" s="26">
-        <v>2010</v>
+        <v>2035</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.2">
@@ -10428,7 +10428,7 @@
   <dimension ref="A1:AA14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:AA13"/>
+      <selection activeCell="A13" sqref="A4:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11434,19 +11434,19 @@
         <v>42</v>
       </c>
       <c r="B13" s="10">
-        <v>1683000</v>
+        <v>0</v>
       </c>
       <c r="C13" s="10">
-        <v>1683000</v>
+        <v>0</v>
       </c>
       <c r="D13" s="10">
-        <v>1683000</v>
+        <v>0</v>
       </c>
       <c r="E13" s="10">
-        <v>1683000</v>
+        <v>0</v>
       </c>
       <c r="F13" s="10">
-        <v>1683000</v>
+        <v>0</v>
       </c>
       <c r="G13" s="10">
         <v>1683000</v>
@@ -11516,35 +11516,35 @@
       <c r="A14" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="25">
-        <v>1280000</v>
-      </c>
-      <c r="C14" s="25">
-        <v>1280000</v>
-      </c>
-      <c r="D14" s="25">
-        <v>1280000</v>
-      </c>
-      <c r="E14" s="25">
-        <v>1280000</v>
-      </c>
-      <c r="F14" s="25">
-        <v>1280000</v>
-      </c>
-      <c r="G14" s="25">
-        <v>1280000</v>
-      </c>
-      <c r="H14" s="25">
-        <v>1280000</v>
-      </c>
-      <c r="I14" s="25">
-        <v>1280000</v>
-      </c>
-      <c r="J14" s="25">
-        <v>1280000</v>
-      </c>
-      <c r="K14" s="25">
-        <v>1280000</v>
+      <c r="B14" s="10">
+        <v>0</v>
+      </c>
+      <c r="C14" s="10">
+        <v>0</v>
+      </c>
+      <c r="D14" s="10">
+        <v>0</v>
+      </c>
+      <c r="E14" s="10">
+        <v>0</v>
+      </c>
+      <c r="F14" s="10">
+        <v>0</v>
+      </c>
+      <c r="G14" s="10">
+        <v>0</v>
+      </c>
+      <c r="H14" s="10">
+        <v>0</v>
+      </c>
+      <c r="I14" s="10">
+        <v>0</v>
+      </c>
+      <c r="J14" s="10">
+        <v>0</v>
+      </c>
+      <c r="K14" s="10">
+        <v>0</v>
       </c>
       <c r="L14" s="25">
         <v>1280000</v>
@@ -11597,6 +11597,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update for production and scrap
</commit_message>
<xml_diff>
--- a/database/Steel Data Mar 10.xlsx
+++ b/database/Steel Data Mar 10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinsupark/jinsu-coding/macc_steel/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A615AE6-A3FE-E445-866E-117A6D317BEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149851FD-EBC5-4549-BC12-439B11C81B69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20020" tabRatio="775" activeTab="4" xr2:uid="{C8B88EB0-6E83-4E76-A7A7-49164EF16775}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20020" tabRatio="775" activeTab="9" xr2:uid="{C8B88EB0-6E83-4E76-A7A7-49164EF16775}"/>
   </bookViews>
   <sheets>
     <sheet name="notes" sheetId="18" r:id="rId1"/>
@@ -1075,8 +1075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED5339A0-3D98-43CE-86F7-53EF60721306}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1110,7 +1110,7 @@
         <v>65</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>2020</v>
@@ -1119,7 +1119,7 @@
         <v>84</v>
       </c>
       <c r="E2">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1127,7 +1127,7 @@
         <v>66</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>2020</v>
@@ -1136,7 +1136,7 @@
         <v>85</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1144,7 +1144,7 @@
         <v>72</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C4">
         <v>2020</v>
@@ -1153,7 +1153,7 @@
         <v>84</v>
       </c>
       <c r="E4">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1161,7 +1161,7 @@
         <v>44</v>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C5">
         <v>2020</v>
@@ -10052,8 +10052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B80F836-AAFA-4D20-813C-A31BE68F85E1}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15:G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10523,7 +10523,7 @@
   <dimension ref="A1:AA18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B14"/>
+      <selection activeCell="B2" sqref="B2:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13082,7 +13082,7 @@
   <dimension ref="A1:AA5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13179,82 +13179,108 @@
         <v>65</v>
       </c>
       <c r="B2" s="16">
-        <v>421098.9</v>
+        <f>capex!B2*0.3</f>
+        <v>150210</v>
       </c>
       <c r="C2" s="16">
-        <v>421098.9</v>
+        <f>capex!C2*0.3</f>
+        <v>150210</v>
       </c>
       <c r="D2" s="16">
-        <v>421098.9</v>
+        <f>capex!D2*0.3</f>
+        <v>150210</v>
       </c>
       <c r="E2" s="16">
-        <v>421098.9</v>
+        <f>capex!E2*0.3</f>
+        <v>150210</v>
       </c>
       <c r="F2" s="16">
-        <v>421098.9</v>
+        <f>capex!F2*0.3</f>
+        <v>150210</v>
       </c>
       <c r="G2" s="16">
-        <v>421098.9</v>
+        <f>capex!G2*0.3</f>
+        <v>150210</v>
       </c>
       <c r="H2" s="16">
-        <v>421098.9</v>
+        <f>capex!H2*0.3</f>
+        <v>150210</v>
       </c>
       <c r="I2" s="16">
-        <v>421098.9</v>
+        <f>capex!I2*0.3</f>
+        <v>150210</v>
       </c>
       <c r="J2" s="16">
-        <v>421098.9</v>
+        <f>capex!J2*0.3</f>
+        <v>150210</v>
       </c>
       <c r="K2" s="16">
-        <v>421098.9</v>
+        <f>capex!K2*0.3</f>
+        <v>150210</v>
       </c>
       <c r="L2" s="16">
-        <v>421098.9</v>
+        <f>capex!L2*0.3</f>
+        <v>150210</v>
       </c>
       <c r="M2" s="16">
-        <v>421098.9</v>
+        <f>capex!M2*0.3</f>
+        <v>150210</v>
       </c>
       <c r="N2" s="16">
-        <v>421098.9</v>
+        <f>capex!N2*0.3</f>
+        <v>150210</v>
       </c>
       <c r="O2" s="16">
-        <v>421098.9</v>
+        <f>capex!O2*0.3</f>
+        <v>150210</v>
       </c>
       <c r="P2" s="16">
-        <v>421098.9</v>
+        <f>capex!P2*0.3</f>
+        <v>150210</v>
       </c>
       <c r="Q2" s="16">
-        <v>421098.9</v>
+        <f>capex!Q2*0.3</f>
+        <v>150210</v>
       </c>
       <c r="R2" s="16">
-        <v>421098.9</v>
+        <f>capex!R2*0.3</f>
+        <v>150210</v>
       </c>
       <c r="S2" s="16">
-        <v>421098.9</v>
+        <f>capex!S2*0.3</f>
+        <v>150210</v>
       </c>
       <c r="T2" s="16">
-        <v>421098.9</v>
+        <f>capex!T2*0.3</f>
+        <v>150210</v>
       </c>
       <c r="U2" s="16">
-        <v>421098.9</v>
+        <f>capex!U2*0.3</f>
+        <v>150210</v>
       </c>
       <c r="V2" s="16">
-        <v>421098.9</v>
+        <f>capex!V2*0.3</f>
+        <v>150210</v>
       </c>
       <c r="W2" s="16">
-        <v>421098.9</v>
+        <f>capex!W2*0.3</f>
+        <v>150210</v>
       </c>
       <c r="X2" s="16">
-        <v>421098.9</v>
+        <f>capex!X2*0.3</f>
+        <v>150210</v>
       </c>
       <c r="Y2" s="16">
-        <v>421098.9</v>
+        <f>capex!Y2*0.3</f>
+        <v>150210</v>
       </c>
       <c r="Z2" s="16">
-        <v>421098.9</v>
+        <f>capex!Z2*0.3</f>
+        <v>150210</v>
       </c>
       <c r="AA2" s="16">
-        <v>421098.9</v>
+        <f>capex!AA2*0.3</f>
+        <v>150210</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="16" x14ac:dyDescent="0.2">
@@ -13262,82 +13288,108 @@
         <v>66</v>
       </c>
       <c r="B3" s="16">
-        <v>357934.065</v>
+        <f>capex!B3*0.3</f>
+        <v>127678.5</v>
       </c>
       <c r="C3" s="16">
-        <v>357934.065</v>
+        <f>capex!C3*0.3</f>
+        <v>127678.5</v>
       </c>
       <c r="D3" s="16">
-        <v>357934.065</v>
+        <f>capex!D3*0.3</f>
+        <v>127678.5</v>
       </c>
       <c r="E3" s="16">
-        <v>357934.065</v>
+        <f>capex!E3*0.3</f>
+        <v>127678.5</v>
       </c>
       <c r="F3" s="16">
-        <v>357934.065</v>
+        <f>capex!F3*0.3</f>
+        <v>127678.5</v>
       </c>
       <c r="G3" s="16">
-        <v>357934.065</v>
+        <f>capex!G3*0.3</f>
+        <v>127678.5</v>
       </c>
       <c r="H3" s="16">
-        <v>357934.065</v>
+        <f>capex!H3*0.3</f>
+        <v>127678.5</v>
       </c>
       <c r="I3" s="16">
-        <v>357934.065</v>
+        <f>capex!I3*0.3</f>
+        <v>127678.5</v>
       </c>
       <c r="J3" s="16">
-        <v>357934.065</v>
+        <f>capex!J3*0.3</f>
+        <v>127678.5</v>
       </c>
       <c r="K3" s="16">
-        <v>357934.065</v>
+        <f>capex!K3*0.3</f>
+        <v>127678.5</v>
       </c>
       <c r="L3" s="16">
-        <v>357934.065</v>
+        <f>capex!L3*0.3</f>
+        <v>127678.5</v>
       </c>
       <c r="M3" s="16">
-        <v>357934.065</v>
+        <f>capex!M3*0.3</f>
+        <v>127678.5</v>
       </c>
       <c r="N3" s="16">
-        <v>357934.065</v>
+        <f>capex!N3*0.3</f>
+        <v>127678.5</v>
       </c>
       <c r="O3" s="16">
-        <v>357934.065</v>
+        <f>capex!O3*0.3</f>
+        <v>127678.5</v>
       </c>
       <c r="P3" s="16">
-        <v>357934.065</v>
+        <f>capex!P3*0.3</f>
+        <v>127678.5</v>
       </c>
       <c r="Q3" s="16">
-        <v>357934.065</v>
+        <f>capex!Q3*0.3</f>
+        <v>127678.5</v>
       </c>
       <c r="R3" s="16">
-        <v>357934.065</v>
+        <f>capex!R3*0.3</f>
+        <v>127678.5</v>
       </c>
       <c r="S3" s="16">
-        <v>357934.065</v>
+        <f>capex!S3*0.3</f>
+        <v>127678.5</v>
       </c>
       <c r="T3" s="16">
-        <v>357934.065</v>
+        <f>capex!T3*0.3</f>
+        <v>127678.5</v>
       </c>
       <c r="U3" s="16">
-        <v>357934.065</v>
+        <f>capex!U3*0.3</f>
+        <v>127678.5</v>
       </c>
       <c r="V3" s="16">
-        <v>357934.065</v>
+        <f>capex!V3*0.3</f>
+        <v>127678.5</v>
       </c>
       <c r="W3" s="16">
-        <v>357934.065</v>
+        <f>capex!W3*0.3</f>
+        <v>127678.5</v>
       </c>
       <c r="X3" s="16">
-        <v>357934.065</v>
+        <f>capex!X3*0.3</f>
+        <v>127678.5</v>
       </c>
       <c r="Y3" s="16">
-        <v>357934.065</v>
+        <f>capex!Y3*0.3</f>
+        <v>127678.5</v>
       </c>
       <c r="Z3" s="16">
-        <v>357934.065</v>
+        <f>capex!Z3*0.3</f>
+        <v>127678.5</v>
       </c>
       <c r="AA3" s="16">
-        <v>357934.065</v>
+        <f>capex!AA3*0.3</f>
+        <v>127678.5</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
@@ -13345,108 +13397,108 @@
         <v>72</v>
       </c>
       <c r="B4" s="16">
-        <f>B2*2</f>
-        <v>842197.8</v>
+        <f>capex!B4*0.3</f>
+        <v>330000</v>
       </c>
       <c r="C4" s="16">
-        <f t="shared" ref="C4:AA4" si="0">C2*2</f>
-        <v>842197.8</v>
+        <f>capex!C4*0.3</f>
+        <v>330000</v>
       </c>
       <c r="D4" s="16">
-        <f t="shared" si="0"/>
-        <v>842197.8</v>
+        <f>capex!D4*0.3</f>
+        <v>330000</v>
       </c>
       <c r="E4" s="16">
-        <f t="shared" si="0"/>
-        <v>842197.8</v>
+        <f>capex!E4*0.3</f>
+        <v>330000</v>
       </c>
       <c r="F4" s="16">
-        <f t="shared" si="0"/>
-        <v>842197.8</v>
+        <f>capex!F4*0.3</f>
+        <v>330000</v>
       </c>
       <c r="G4" s="16">
-        <f t="shared" si="0"/>
-        <v>842197.8</v>
+        <f>capex!G4*0.3</f>
+        <v>330000</v>
       </c>
       <c r="H4" s="16">
-        <f t="shared" si="0"/>
-        <v>842197.8</v>
+        <f>capex!H4*0.3</f>
+        <v>323400</v>
       </c>
       <c r="I4" s="16">
-        <f t="shared" si="0"/>
-        <v>842197.8</v>
+        <f>capex!I4*0.3</f>
+        <v>316932</v>
       </c>
       <c r="J4" s="16">
-        <f t="shared" si="0"/>
-        <v>842197.8</v>
+        <f>capex!J4*0.3</f>
+        <v>310593.36</v>
       </c>
       <c r="K4" s="16">
-        <f t="shared" si="0"/>
-        <v>842197.8</v>
+        <f>capex!K4*0.3</f>
+        <v>304381.49279999995</v>
       </c>
       <c r="L4" s="16">
-        <f t="shared" si="0"/>
-        <v>842197.8</v>
+        <f>capex!L4*0.3</f>
+        <v>298293.86294399993</v>
       </c>
       <c r="M4" s="16">
-        <f t="shared" si="0"/>
-        <v>842197.8</v>
+        <f>capex!M4*0.3</f>
+        <v>292327.98568511993</v>
       </c>
       <c r="N4" s="16">
-        <f t="shared" si="0"/>
-        <v>842197.8</v>
+        <f>capex!N4*0.3</f>
+        <v>286481.42597141751</v>
       </c>
       <c r="O4" s="16">
-        <f t="shared" si="0"/>
-        <v>842197.8</v>
+        <f>capex!O4*0.3</f>
+        <v>280751.79745198914</v>
       </c>
       <c r="P4" s="16">
-        <f t="shared" si="0"/>
-        <v>842197.8</v>
+        <f>capex!P4*0.3</f>
+        <v>275136.76150294935</v>
       </c>
       <c r="Q4" s="16">
-        <f t="shared" si="0"/>
-        <v>842197.8</v>
+        <f>capex!Q4*0.3</f>
+        <v>269634.02627289039</v>
       </c>
       <c r="R4" s="16">
-        <f t="shared" si="0"/>
-        <v>842197.8</v>
+        <f>capex!R4*0.3</f>
+        <v>264241.34574743256</v>
       </c>
       <c r="S4" s="16">
-        <f t="shared" si="0"/>
-        <v>842197.8</v>
+        <f>capex!S4*0.3</f>
+        <v>258956.51883248394</v>
       </c>
       <c r="T4" s="16">
-        <f t="shared" si="0"/>
-        <v>842197.8</v>
+        <f>capex!T4*0.3</f>
+        <v>253777.38845583427</v>
       </c>
       <c r="U4" s="16">
-        <f t="shared" si="0"/>
-        <v>842197.8</v>
+        <f>capex!U4*0.3</f>
+        <v>248701.84068671757</v>
       </c>
       <c r="V4" s="16">
-        <f t="shared" si="0"/>
-        <v>842197.8</v>
+        <f>capex!V4*0.3</f>
+        <v>243727.8038729832</v>
       </c>
       <c r="W4" s="16">
-        <f t="shared" si="0"/>
-        <v>842197.8</v>
+        <f>capex!W4*0.3</f>
+        <v>238853.24779552355</v>
       </c>
       <c r="X4" s="16">
-        <f t="shared" si="0"/>
-        <v>842197.8</v>
+        <f>capex!X4*0.3</f>
+        <v>234076.18283961309</v>
       </c>
       <c r="Y4" s="16">
-        <f t="shared" si="0"/>
-        <v>842197.8</v>
+        <f>capex!Y4*0.3</f>
+        <v>229394.65918282082</v>
       </c>
       <c r="Z4" s="16">
-        <f t="shared" si="0"/>
-        <v>842197.8</v>
+        <f>capex!Z4*0.3</f>
+        <v>224806.7659991644</v>
       </c>
       <c r="AA4" s="16">
-        <f t="shared" si="0"/>
-        <v>842197.8</v>
+        <f>capex!AA4*0.3</f>
+        <v>220310.63067918111</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
@@ -13454,82 +13506,108 @@
         <v>44</v>
       </c>
       <c r="B5" s="16">
-        <v>185299.77</v>
+        <f>capex!B5*0.3</f>
+        <v>120000</v>
       </c>
       <c r="C5" s="16">
-        <v>185299.77</v>
+        <f>capex!C5*0.3</f>
+        <v>120000</v>
       </c>
       <c r="D5" s="16">
-        <v>185299.77</v>
+        <f>capex!D5*0.3</f>
+        <v>120000</v>
       </c>
       <c r="E5" s="16">
-        <v>185299.77</v>
+        <f>capex!E5*0.3</f>
+        <v>120000</v>
       </c>
       <c r="F5" s="16">
-        <v>185299.77</v>
+        <f>capex!F5*0.3</f>
+        <v>120000</v>
       </c>
       <c r="G5" s="16">
-        <v>185299.77</v>
+        <f>capex!G5*0.3</f>
+        <v>120000</v>
       </c>
       <c r="H5" s="16">
-        <v>185299.77</v>
+        <f>capex!H5*0.3</f>
+        <v>120000</v>
       </c>
       <c r="I5" s="16">
-        <v>185299.77</v>
+        <f>capex!I5*0.3</f>
+        <v>120000</v>
       </c>
       <c r="J5" s="16">
-        <v>185299.77</v>
+        <f>capex!J5*0.3</f>
+        <v>120000</v>
       </c>
       <c r="K5" s="16">
-        <v>185299.77</v>
+        <f>capex!K5*0.3</f>
+        <v>120000</v>
       </c>
       <c r="L5" s="16">
-        <v>185299.77</v>
+        <f>capex!L5*0.3</f>
+        <v>120000</v>
       </c>
       <c r="M5" s="16">
-        <v>185299.77</v>
+        <f>capex!M5*0.3</f>
+        <v>120000</v>
       </c>
       <c r="N5" s="16">
-        <v>185299.77</v>
+        <f>capex!N5*0.3</f>
+        <v>120000</v>
       </c>
       <c r="O5" s="16">
-        <v>185299.77</v>
+        <f>capex!O5*0.3</f>
+        <v>120000</v>
       </c>
       <c r="P5" s="16">
-        <v>185299.77</v>
+        <f>capex!P5*0.3</f>
+        <v>120000</v>
       </c>
       <c r="Q5" s="16">
-        <v>185299.77</v>
+        <f>capex!Q5*0.3</f>
+        <v>120000</v>
       </c>
       <c r="R5" s="16">
-        <v>185299.77</v>
+        <f>capex!R5*0.3</f>
+        <v>120000</v>
       </c>
       <c r="S5" s="16">
-        <v>185299.77</v>
+        <f>capex!S5*0.3</f>
+        <v>120000</v>
       </c>
       <c r="T5" s="16">
-        <v>185299.77</v>
+        <f>capex!T5*0.3</f>
+        <v>120000</v>
       </c>
       <c r="U5" s="16">
-        <v>185299.77</v>
+        <f>capex!U5*0.3</f>
+        <v>120000</v>
       </c>
       <c r="V5" s="16">
-        <v>185299.77</v>
+        <f>capex!V5*0.3</f>
+        <v>120000</v>
       </c>
       <c r="W5" s="16">
-        <v>185299.77</v>
+        <f>capex!W5*0.3</f>
+        <v>120000</v>
       </c>
       <c r="X5" s="16">
-        <v>185299.77</v>
+        <f>capex!X5*0.3</f>
+        <v>120000</v>
       </c>
       <c r="Y5" s="16">
-        <v>185299.77</v>
+        <f>capex!Y5*0.3</f>
+        <v>120000</v>
       </c>
       <c r="Z5" s="16">
-        <v>185299.77</v>
+        <f>capex!Z5*0.3</f>
+        <v>120000</v>
       </c>
       <c r="AA5" s="16">
-        <v>185299.77</v>
+        <f>capex!AA5*0.3</f>
+        <v>120000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>